<commit_message>
Modificaciones en el informe y DimReduction
</commit_message>
<xml_diff>
--- a/informe/tables/Clustering.xlsx
+++ b/informe/tables/Clustering.xlsx
@@ -1,166 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Projects\MangoGrading\informe\tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8C47E4-EF7B-42C5-B3CB-E7C8B0208EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
-  <si>
-    <t>base model</t>
-  </si>
-  <si>
-    <t>algorithm</t>
-  </si>
-  <si>
-    <t>accuracy</t>
-  </si>
-  <si>
-    <t>eval time</t>
-  </si>
-  <si>
-    <t>10/04/2022 23:25:06</t>
-  </si>
-  <si>
-    <t>inception</t>
-  </si>
-  <si>
-    <t>KMeans</t>
-  </si>
-  <si>
-    <t>10/04/2022 23:30:20</t>
-  </si>
-  <si>
-    <t>vgg</t>
-  </si>
-  <si>
-    <t>10/04/2022 23:39:06</t>
-  </si>
-  <si>
-    <t>xception</t>
-  </si>
-  <si>
-    <t>10/04/2022 23:51:51</t>
-  </si>
-  <si>
-    <t>resnet</t>
-  </si>
-  <si>
-    <t>06/05/2022 14:33:28</t>
-  </si>
-  <si>
-    <t>06/05/2022 15:27:01</t>
-  </si>
-  <si>
-    <t>hog</t>
-  </si>
-  <si>
-    <t>06/05/2022 15:32:32</t>
-  </si>
-  <si>
-    <t>rgb</t>
-  </si>
-  <si>
-    <t>06/05/2022 16:18:08</t>
-  </si>
-  <si>
-    <t>decision_tree</t>
-  </si>
-  <si>
-    <t>06/05/2022 16:21:49</t>
-  </si>
-  <si>
-    <t>06/05/2022 16:28:47</t>
-  </si>
-  <si>
-    <t>08/05/2022 14:09:08</t>
-  </si>
-  <si>
-    <t>spectral</t>
-  </si>
-  <si>
-    <t>08/05/2022 14:11:41</t>
-  </si>
-  <si>
-    <t>08/05/2022 14:14:55</t>
-  </si>
-  <si>
-    <t>08/05/2022 18:43:25</t>
-  </si>
-  <si>
-    <t>multiprocess</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="8">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -265,45 +174,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -569,320 +546,444 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.42578125" bestFit="1" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>base model</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>algorithm</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>eval time</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>multiprocess</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>10/04/2022 23:25:06</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>inception</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>0.38</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>145.44</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>10/04/2022 23:30:20</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>vgg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>0.6</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>234.82</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E4">
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>10/04/2022 23:39:06</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>xception</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="E4" t="n">
         <v>188.29</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>10/04/2022 23:51:51</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>resnet</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>0.18</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>196.06</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>06/05/2022 14:33:28</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>vgg</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>0.6</v>
       </c>
-      <c r="E6">
-        <v>270.39999999999998</v>
+      <c r="E6" t="n">
+        <v>270.4</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>06/05/2022 15:27:01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>hog</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>0.36</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>12.33</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>06/05/2022 15:32:32</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>rgb</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>KMeans</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>0.27</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>16.22</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>06/05/2022 16:18:08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>hog</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>decision_tree</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>0.4</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>54.37</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>06/05/2022 16:21:49</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>rgb</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>decision_tree</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>0.41</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>45.07</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E11">
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>06/05/2022 16:28:47</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>vgg</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>decision_tree</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E11" t="n">
         <v>273.32</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12">
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>08/05/2022 14:09:08</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>vgg</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>spectral</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>0.3</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>202.47</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13">
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>08/05/2022 14:11:41</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>hog</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>spectral</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>0.33</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>56.63</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14">
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>08/05/2022 14:14:55</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>rgb</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>spectral</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>0.3</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>6.53</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15">
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>08/05/2022 18:43:25</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>hog</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>spectral</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>0.33</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>41.8</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>10/05/2022 10:26:39</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>pca</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>decision_tree</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="E16" t="n">
+        <v>43.94</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>